<commit_message>
up to task 4 is now done and plots formatted
</commit_message>
<xml_diff>
--- a/airJetLab.xlsx
+++ b/airJetLab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://computingservices-my.sharepoint.com/personal/mci28_bath_ac_uk/Documents/thermofluids/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\MATLAB\airJetLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81B6FB44-A682-49B3-96E9-4C0AF0C0C850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E162F887-038B-4FC3-B103-983462A126CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5673A605-1398-4521-B3E4-DF8ADFB7E050}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5673A605-1398-4521-B3E4-DF8ADFB7E050}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>axial distance</t>
   </si>
@@ -65,16 +65,22 @@
     <t>x = 300 mm (10D)</t>
   </si>
   <si>
-    <t>R (mm)</t>
+    <t>V</t>
   </si>
   <si>
-    <t>L (mm)</t>
+    <t xml:space="preserve">R </t>
   </si>
   <si>
-    <t>H (mm)</t>
+    <t xml:space="preserve">L </t>
   </si>
   <si>
-    <t>V</t>
+    <t>H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H </t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -448,16 +454,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E8AA4D-D77D-47F4-B237-BE02E0078146}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +495,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -521,7 +527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -562,7 +568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -603,7 +609,7 @@
         <v>5.9766226717619206</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -611,7 +617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -619,7 +625,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -630,45 +636,45 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
         <v>9</v>
       </c>
-      <c r="G14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" t="s">
         <v>11</v>
       </c>
-      <c r="I14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" t="s">
         <v>9</v>
       </c>
-      <c r="L14" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" t="s">
-        <v>11</v>
-      </c>
-      <c r="N14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>28</v>
       </c>
@@ -679,9 +685,9 @@
         <f>B15-$B$8</f>
         <v>-1</v>
       </c>
-      <c r="D15">
-        <f>40*SQRT(SIN(0.2251474735)*10*ABS(C15)/1000)</f>
-        <v>1.8899740358168575</v>
+      <c r="D15" t="e">
+        <f>40*SQRT(SIN(0.2251474735)*10*C15/1000)</f>
+        <v>#NUM!</v>
       </c>
       <c r="F15">
         <v>50</v>
@@ -693,9 +699,9 @@
         <f>G15-$B$8</f>
         <v>-1</v>
       </c>
-      <c r="I15">
-        <f>40*SQRT(SIN(0.2251474735)*10*ABS(H15)/1000)</f>
-        <v>1.8899740358168575</v>
+      <c r="I15" t="e">
+        <f>40*SQRT(SIN(0.2251474735)*10*H15/1000)</f>
+        <v>#NUM!</v>
       </c>
       <c r="K15">
         <v>60</v>
@@ -707,12 +713,12 @@
         <f>L15-$B$8</f>
         <v>-1</v>
       </c>
-      <c r="N15">
-        <f>40*SQRT(SIN(0.2251474735)*10*ABS(M15)/1000)</f>
-        <v>1.8899740358168575</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N15" t="e">
+        <f>40*SQRT(SIN(0.2251474735)*10*M15/1000)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>24</v>
       </c>
@@ -723,9 +729,9 @@
         <f t="shared" ref="C16:C29" si="2">B16-$B$8</f>
         <v>-1</v>
       </c>
-      <c r="D16">
-        <f t="shared" ref="D16:D29" si="3">40*SQRT(SIN(0.2251474735)*10*ABS(C16)/1000)</f>
-        <v>1.8899740358168575</v>
+      <c r="D16" t="e">
+        <f t="shared" ref="D16:D29" si="3">40*SQRT(SIN(0.2251474735)*10*C16/1000)</f>
+        <v>#NUM!</v>
       </c>
       <c r="F16">
         <v>45</v>
@@ -737,9 +743,9 @@
         <f t="shared" ref="H16:H35" si="4">G16-$B$8</f>
         <v>-1</v>
       </c>
-      <c r="I16">
-        <f t="shared" ref="I16:I35" si="5">40*SQRT(SIN(0.2251474735)*10*ABS(H16)/1000)</f>
-        <v>1.8899740358168575</v>
+      <c r="I16" t="e">
+        <f t="shared" ref="I16:I35" si="5">40*SQRT(SIN(0.2251474735)*10*H16/1000)</f>
+        <v>#NUM!</v>
       </c>
       <c r="K16">
         <v>55</v>
@@ -751,12 +757,12 @@
         <f t="shared" ref="M16:M39" si="6">L16-$B$8</f>
         <v>-1</v>
       </c>
-      <c r="N16">
-        <f t="shared" ref="N16:N39" si="7">40*SQRT(SIN(0.2251474735)*10*ABS(M16)/1000)</f>
-        <v>1.8899740358168575</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N16" t="e">
+        <f t="shared" ref="N16:N39" si="7">40*SQRT(SIN(0.2251474735)*10*M16/1000)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>20</v>
       </c>
@@ -781,9 +787,9 @@
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="5"/>
-        <v>1.8899740358168575</v>
+      <c r="I17" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
       </c>
       <c r="K17">
         <v>50</v>
@@ -795,12 +801,12 @@
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="7"/>
-        <v>1.8899740358168575</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N17" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -825,9 +831,9 @@
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="5"/>
-        <v>1.8899740358168575</v>
+      <c r="I18" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
       </c>
       <c r="K18">
         <v>45</v>
@@ -839,12 +845,12 @@
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
-      <c r="N18">
-        <f t="shared" si="7"/>
-        <v>1.8899740358168575</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N18" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>12</v>
       </c>
@@ -883,12 +889,12 @@
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
-      <c r="N19">
-        <f t="shared" si="7"/>
-        <v>1.8899740358168575</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N19" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>8</v>
       </c>
@@ -932,7 +938,7 @@
         <v>1.8899740358168575</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>4</v>
       </c>
@@ -976,7 +982,7 @@
         <v>3.2735310550207988</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1020,7 +1026,7 @@
         <v>5.0004012831404863</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>-4</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>6.2683347403182346</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>-8</v>
       </c>
@@ -1108,7 +1114,7 @@
         <v>7.0716353119251032</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>-12</v>
       </c>
@@ -1152,7 +1158,7 @@
         <v>8.4522208395922309</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>-16</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>9.4498701790842894</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>-20</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>10.000802566280973</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>-24</v>
       </c>
@@ -1284,7 +1290,7 @@
         <v>10.000802566280973</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>-28</v>
       </c>
@@ -1295,9 +1301,9 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="e">
         <f t="shared" si="3"/>
-        <v>1.8899740358168575</v>
+        <v>#NUM!</v>
       </c>
       <c r="F29">
         <v>-20</v>
@@ -1328,7 +1334,7 @@
         <v>9.4498701790842894</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F30">
         <v>-25</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>8.4522208395922309</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F31">
         <v>-30</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>7.5598961432674301</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F32">
         <v>-35</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>6.2683347403182346</v>
       </c>
     </row>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F33">
         <v>-40</v>
       </c>
@@ -1429,9 +1435,9 @@
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="5"/>
-        <v>1.8899740358168575</v>
+      <c r="I33" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
       </c>
       <c r="K33">
         <v>-30</v>
@@ -1448,7 +1454,7 @@
         <v>5.0004012831404863</v>
       </c>
     </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F34">
         <v>-45</v>
       </c>
@@ -1459,9 +1465,9 @@
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
-      <c r="I34">
-        <f t="shared" si="5"/>
-        <v>1.8899740358168575</v>
+      <c r="I34" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
       </c>
       <c r="K34">
         <v>-35</v>
@@ -1478,7 +1484,7 @@
         <v>3.779948071633715</v>
       </c>
     </row>
-    <row r="35" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F35">
         <v>-50</v>
       </c>
@@ -1489,9 +1495,9 @@
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
-      <c r="I35">
-        <f t="shared" si="5"/>
-        <v>1.8899740358168575</v>
+      <c r="I35" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
       </c>
       <c r="K35">
         <v>-40</v>
@@ -1508,7 +1514,7 @@
         <v>2.6728269139852139</v>
       </c>
     </row>
-    <row r="36" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:14" x14ac:dyDescent="0.35">
       <c r="K36">
         <v>-45</v>
       </c>
@@ -1524,7 +1530,7 @@
         <v>1.8899740358168575</v>
       </c>
     </row>
-    <row r="37" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:14" x14ac:dyDescent="0.35">
       <c r="K37">
         <v>-50</v>
       </c>
@@ -1540,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:14" x14ac:dyDescent="0.35">
       <c r="K38">
         <v>-55</v>
       </c>
@@ -1556,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:14" x14ac:dyDescent="0.35">
       <c r="K39">
         <v>-60</v>
       </c>
@@ -1567,9 +1573,9 @@
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
-      <c r="N39">
-        <f t="shared" si="7"/>
-        <v>1.8899740358168575</v>
+      <c r="N39" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>